<commit_message>
Toevoeging aan takenverdeling DAL
Status column toegevoegd
</commit_message>
<xml_diff>
--- a/Doc/TakenVerdeling/DALmethodes.xlsx
+++ b/Doc/TakenVerdeling/DALmethodes.xlsx
@@ -22,6 +22,9 @@
     <t>Auteur</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>DaOrganism</t>
   </si>
   <si>
@@ -31,10 +34,16 @@
     <t>Bert</t>
   </si>
   <si>
-    <t>selectOneById()</t>
-  </si>
-  <si>
-    <t>Bert</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>selectOneById()</t>
+  </si>
+  <si>
+    <t>Bert</t>
+  </si>
+  <si>
+    <t>Working</t>
   </si>
   <si>
     <t>selectAllByNameLike()</t>
@@ -332,13 +341,21 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left/>
@@ -352,16 +369,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="2">
       <alignment/>
     </xf>
   </cellXfs>
@@ -397,427 +414,436 @@
       <c t="s" s="2" r="C1">
         <v>2</v>
       </c>
+      <c t="s" s="2" r="D1">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c t="s" s="3" r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c t="s" s="4" r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c t="s" s="4" r="C2">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c t="s" s="4" r="D2">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="4" r="B3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c t="s" s="4" r="C3">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c t="s" s="4" r="D3">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="4" r="B4">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c t="s" s="4" r="C4">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="4" r="B5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c t="s" s="4" r="C5">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="4" r="B6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c t="s" s="4" r="C6">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="4" r="B7">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c t="s" s="4" r="C7">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="4" r="B8">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c t="s" s="4" r="C8">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="4" r="B9">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c t="s" s="4" r="C9">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="4" r="B10">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c t="s" s="4" r="C10">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="4" r="B11">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c t="s" s="4" r="C11">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="4" r="B12">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c t="s" s="4" r="C12">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="4" r="B13">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c t="s" s="4" r="C13">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="3" r="A14">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c t="s" s="4" r="B14">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c t="s" s="4" r="C14">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="4" r="B15">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c t="s" s="4" r="C15">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="4" r="B16">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c t="s" s="4" r="C16">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="4" r="B17">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c t="s" s="4" r="C17">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="4" r="B18">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c t="s" s="4" r="C18">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="4" r="B19">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c t="s" s="4" r="C19">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="3" r="A20">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c t="s" s="4" r="B20">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="4" r="B21">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22">
       <c t="s" s="4" r="B22">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23">
       <c t="s" s="4" r="B23">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24">
       <c t="s" s="4" r="B24">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="4" r="A25">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c t="s" s="4" r="B25">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26">
       <c t="s" s="4" r="B26">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27">
       <c t="s" s="4" r="B27">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="4" r="B28">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="4" r="B29">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="4" r="B30">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31">
       <c t="s" s="4" r="A31">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c t="s" s="4" r="B31">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="4" r="B32">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="4" r="B33">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="4" r="B34">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="4" r="B35">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36">
       <c t="s" s="4" r="B36">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37">
       <c t="s" s="4" r="A37">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c t="s" s="4" r="B37">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38">
       <c t="s" s="4" r="B38">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39">
       <c t="s" s="4" r="B39">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40">
       <c t="s" s="4" r="B40">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41">
       <c t="s" s="4" r="B41">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42">
       <c t="s" s="4" r="B42">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43">
       <c t="s" s="4" r="A43">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c t="s" s="4" r="B43">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44">
       <c t="s" s="4" r="B44">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45">
       <c t="s" s="4" r="B45">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46">
       <c t="s" s="4" r="B46">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47">
       <c t="s" s="4" r="B47">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48">
       <c t="s" s="4" r="A48">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c t="s" s="4" r="B48">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49">
       <c t="s" s="4" r="B49">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50">
       <c t="s" s="4" r="B50">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51">
       <c t="s" s="4" r="B51">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52">
       <c t="s" s="4" r="B52">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53">
       <c t="s" s="4" r="A53">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c t="s" s="4" r="B53">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54">
       <c t="s" s="4" r="B54">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55">
       <c t="s" s="4" r="B55">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56">
       <c t="s" s="4" r="B56">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57">
       <c t="s" s="4" r="B57">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58">
       <c t="s" s="4" r="A58">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c t="s" s="4" r="B58">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59">
       <c t="s" s="4" r="B59">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60">
       <c t="s" s="4" r="B60">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61">
       <c t="s" s="4" r="B61">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62">
       <c t="s" s="4" r="B62">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63">
       <c t="s" s="4" r="B63">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64">
       <c t="s" s="4" r="A64">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c t="s" s="4" r="B64">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65">
       <c t="s" s="4" r="B65">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66">
       <c t="s" s="4" r="B66">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67">
       <c t="s" s="4" r="B67">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68">
       <c t="s" s="4" r="B68">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DAL useraccount gekozen + DB gewijzigd
- season_id verwijderd uit organism tabel

- first_name in user_accounts tabel NOT NULL gemaakt. Alleen maar een
achternaam komt onvolledig over.

- email in user_accounts tabel UNIQUE gemaakt. Men kan niet dezelfde
e-mail voor meerdere accounts gebruiken.

- phone in user_accounts tabel van INT naar STRING gewijzigd. Nullen
vooraan worden afgekapt omdat het geen relevante informatie is, numeriek
gezien.

- phone in user_accounts tabel mag NULL zijn. Niet iedereen wilt zijn
nummer beschikbaar stellen of heeft zelfs een GSM.

- address verwijderd uit user_accounts tabel. Onze website vereist zo'n
specificiteit niet. City/country is genoeg. Voor contact gebruik je
telefoonnummer (of eventuel private message systeem).
</commit_message>
<xml_diff>
--- a/Doc/TakenVerdeling/DALmethodes.xlsx
+++ b/Doc/TakenVerdeling/DALmethodes.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Blad1" state="visible" r:id="rId3"/>
+    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="104">
   <si>
     <t>DAL klasse</t>
   </si>
@@ -317,28 +323,39 @@
   </si>
   <si>
     <t>update()</t>
+  </si>
+  <si>
+    <t>Oualid</t>
+  </si>
+  <si>
+    <t>Lenny??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="3">
@@ -356,493 +373,847 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="2">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="2">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+  <a:themeElements>
+    <a:clrScheme name="Kantoor">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Kantoor">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Kantoor">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="22.0"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="2" r="B1">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="2" r="C1">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="D1">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="3" r="A2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="4" r="B2">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="4" r="C2">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="4" r="D2">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="4" r="B3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="4" r="C3">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="4" r="D3">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" s="4" r="B4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="4" r="C4">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" s="4" r="B5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="4" r="C5">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" s="4" r="B6">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="4" r="C6">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" s="4" r="B7">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="4" r="C7">
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" s="4" r="B8">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="4" r="C8">
+      <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" s="4" r="B9">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A9" s="6"/>
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="4" r="C9">
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" s="4" r="B10">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A10" s="6"/>
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="4" r="C10">
+      <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" s="4" r="B11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A11" s="6"/>
+      <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="4" r="C11">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" s="4" r="B12">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A12" s="6"/>
+      <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="4" r="C12">
+      <c r="C12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13">
-      <c t="s" s="4" r="B13">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A13" s="6"/>
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="4" r="C13">
+      <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14">
-      <c t="s" s="3" r="A14">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="4" r="B14">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="4" r="C14">
+      <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15">
-      <c t="s" s="4" r="B15">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A15" s="6"/>
+      <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="4" r="C15">
+      <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" s="4" r="B16">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A16" s="6"/>
+      <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="4" r="C16">
+      <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" s="4" r="B17">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A17" s="6"/>
+      <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="4" r="C17">
+      <c r="C17" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18">
-      <c t="s" s="4" r="B18">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="4" r="C18">
+      <c r="C18" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19">
-      <c t="s" s="4" r="B19">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A19" s="6"/>
+      <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="4" r="C19">
+      <c r="C19" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20">
-      <c t="s" s="3" r="A20">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="4" r="B20">
+      <c r="B20" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21">
-      <c t="s" s="4" r="B21">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A21" s="6"/>
+      <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22">
-      <c t="s" s="4" r="B22">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A22" s="6"/>
+      <c r="B22" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23">
-      <c t="s" s="4" r="B23">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A23" s="6"/>
+      <c r="B23" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24">
-      <c t="s" s="4" r="B24">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A24" s="6"/>
+      <c r="B24" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25">
-      <c t="s" s="4" r="A25">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A25" s="3" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="4" r="B25">
+      <c r="B25" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26">
-      <c t="s" s="4" r="B26">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B26" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27">
-      <c t="s" s="4" r="B27">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B27" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28">
-      <c t="s" s="4" r="B28">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B28" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29">
-      <c t="s" s="4" r="B29">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30">
-      <c t="s" s="4" r="B30">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B30" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31">
-      <c t="s" s="4" r="A31">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A31" s="3" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="4" r="B31">
+      <c r="B31" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32">
-      <c t="s" s="4" r="B32">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B32" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33">
-      <c t="s" s="4" r="B33">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B33" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34">
-      <c t="s" s="4" r="B34">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B34" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35">
-      <c t="s" s="4" r="B35">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B35" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36">
-      <c t="s" s="4" r="B36">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B36" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="37">
-      <c t="s" s="4" r="A37">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A37" s="3" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="4" r="B37">
+      <c r="B37" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38">
-      <c t="s" s="4" r="B38">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B38" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39">
-      <c t="s" s="4" r="B39">
+    <row r="39" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B39" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40">
-      <c t="s" s="4" r="B40">
+    <row r="40" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B40" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="41">
-      <c t="s" s="4" r="B41">
+    <row r="41" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B41" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42">
-      <c t="s" s="4" r="B42">
+    <row r="42" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B42" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43">
-      <c t="s" s="4" r="A43">
+    <row r="43" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A43" s="3" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="4" r="B43">
+      <c r="B43" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="44">
-      <c t="s" s="4" r="B44">
+    <row r="44" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B44" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="45">
-      <c t="s" s="4" r="B45">
+    <row r="45" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B45" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="46">
-      <c t="s" s="4" r="B46">
+    <row r="46" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B46" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="47">
-      <c t="s" s="4" r="B47">
+    <row r="47" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B47" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="48">
-      <c t="s" s="4" r="A48">
+    <row r="48" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A48" s="3" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="4" r="B48">
+      <c r="B48" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="49">
-      <c t="s" s="4" r="B49">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B49" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50">
-      <c t="s" s="4" r="B50">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B50" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="51">
-      <c t="s" s="4" r="B51">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B51" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52">
-      <c t="s" s="4" r="B52">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B52" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53">
-      <c t="s" s="4" r="A53">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A53" s="3" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="4" r="B53">
+      <c r="B53" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54">
-      <c t="s" s="4" r="B54">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B54" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55">
-      <c t="s" s="4" r="B55">
+    <row r="55" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B55" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="56">
-      <c t="s" s="4" r="B56">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B56" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57">
-      <c t="s" s="4" r="B57">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B57" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="58">
-      <c t="s" s="4" r="A58">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A58" s="3" t="s">
         <v>89</v>
       </c>
-      <c t="s" s="4" r="B58">
+      <c r="B58" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="59">
-      <c t="s" s="4" r="B59">
+      <c r="C58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B59" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="60">
-      <c t="s" s="4" r="B60">
+      <c r="C59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B60" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="61">
-      <c t="s" s="4" r="B61">
+      <c r="C60" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B61" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="62">
-      <c t="s" s="4" r="B62">
+      <c r="C61" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B62" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="63">
-      <c t="s" s="4" r="B63">
+      <c r="C62" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B63" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="64">
-      <c t="s" s="4" r="A64">
+      <c r="C63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A64" s="3" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="4" r="B64">
+      <c r="B64" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="65">
-      <c t="s" s="4" r="B65">
+    <row r="65" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B65" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="66">
-      <c t="s" s="4" r="B66">
+    <row r="66" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B66" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67">
-      <c t="s" s="4" r="B67">
+    <row r="67" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B67" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="68">
-      <c t="s" s="4" r="B68">
+    <row r="68" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B68" s="3" t="s">
         <v>101</v>
       </c>
     </row>
@@ -852,6 +1223,6 @@
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A2:A13"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
methodes toegevoegd bij useraccounts
spreekt voor zich
</commit_message>
<xml_diff>
--- a/Doc/TakenVerdeling/DALmethodes.xlsx
+++ b/Doc/TakenVerdeling/DALmethodes.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lennyasus\Documents\GitHub\ProjectOman\Doc\TakenVerdeling\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Blad1" state="visible" r:id="rId3"/>
+    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t>DAL klasse</t>
   </si>
@@ -298,47 +306,55 @@
     <t>delete()</t>
   </si>
   <si>
+    <t>DaSeason</t>
+  </si>
+  <si>
+    <t>SelectAll()</t>
+  </si>
+  <si>
+    <t>selectOneById()</t>
+  </si>
+  <si>
+    <t>insert()</t>
+  </si>
+  <si>
+    <t>delete()</t>
+  </si>
+  <si>
     <t>update()</t>
   </si>
   <si>
-    <t>DaSeason</t>
-  </si>
-  <si>
-    <t>SelectAll()</t>
-  </si>
-  <si>
-    <t>selectOneById()</t>
-  </si>
-  <si>
-    <t>insert()</t>
-  </si>
-  <si>
-    <t>delete()</t>
-  </si>
-  <si>
-    <t>update()</t>
+    <t>checkUsernamePassword()</t>
+  </si>
+  <si>
+    <t>updatePassword()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="3">
@@ -356,494 +372,792 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="2">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="2">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="22.0"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="2" r="B1">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="2" r="C1">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="D1">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="3" r="A2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="4" r="B2">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="4" r="C2">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="4" r="D2">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="4" r="B3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="4" r="C3">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="4" r="D3">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" s="4" r="B4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="4" r="C4">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" s="4" r="B5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="4" r="C5">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" s="4" r="B6">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="4" r="C6">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" s="4" r="B7">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="4" r="C7">
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" s="4" r="B8">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="4" r="C8">
+      <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" s="4" r="B9">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="4" r="C9">
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" s="4" r="B10">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="4" r="C10">
+      <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" s="4" r="B11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="4" r="C11">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" s="4" r="B12">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="4" r="C12">
+      <c r="C12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13">
-      <c t="s" s="4" r="B13">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="4" r="C13">
+      <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14">
-      <c t="s" s="3" r="A14">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="4" r="B14">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="4" r="C14">
+      <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15">
-      <c t="s" s="4" r="B15">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="4" r="C15">
+      <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" s="4" r="B16">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="4" r="C16">
+      <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" s="4" r="B17">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="4" r="C17">
+      <c r="C17" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18">
-      <c t="s" s="4" r="B18">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="4" r="C18">
+      <c r="C18" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19">
-      <c t="s" s="4" r="B19">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="4" r="C19">
+      <c r="C19" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20">
-      <c t="s" s="3" r="A20">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="4" r="B20">
+      <c r="B20" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21">
-      <c t="s" s="4" r="B21">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22">
-      <c t="s" s="4" r="B22">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23">
-      <c t="s" s="4" r="B23">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24">
-      <c t="s" s="4" r="B24">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25">
-      <c t="s" s="4" r="A25">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="4" r="B25">
+      <c r="B25" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26">
-      <c t="s" s="4" r="B26">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27">
-      <c t="s" s="4" r="B27">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28">
-      <c t="s" s="4" r="B28">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29">
-      <c t="s" s="4" r="B29">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30">
-      <c t="s" s="4" r="B30">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31">
-      <c t="s" s="4" r="A31">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="4" r="B31">
+      <c r="B31" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32">
-      <c t="s" s="4" r="B32">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33">
-      <c t="s" s="4" r="B33">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34">
-      <c t="s" s="4" r="B34">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35">
-      <c t="s" s="4" r="B35">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36">
-      <c t="s" s="4" r="B36">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="37">
-      <c t="s" s="4" r="A37">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="4" r="B37">
+      <c r="B37" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38">
-      <c t="s" s="4" r="B38">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39">
-      <c t="s" s="4" r="B39">
+    <row r="39" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B39" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40">
-      <c t="s" s="4" r="B40">
+    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="41">
-      <c t="s" s="4" r="B41">
+    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42">
-      <c t="s" s="4" r="B42">
+    <row r="42" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43">
-      <c t="s" s="4" r="A43">
+    <row r="43" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="4" r="B43">
+      <c r="B43" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="44">
-      <c t="s" s="4" r="B44">
+    <row r="44" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="45">
-      <c t="s" s="4" r="B45">
+    <row r="45" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="46">
-      <c t="s" s="4" r="B46">
+    <row r="46" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B46" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="47">
-      <c t="s" s="4" r="B47">
+    <row r="47" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B47" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="48">
-      <c t="s" s="4" r="A48">
+    <row r="48" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="4" r="B48">
+      <c r="B48" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="49">
-      <c t="s" s="4" r="B49">
+    <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B49" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50">
-      <c t="s" s="4" r="B50">
+    <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B50" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="51">
-      <c t="s" s="4" r="B51">
+    <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B51" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52">
-      <c t="s" s="4" r="B52">
+    <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B52" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53">
-      <c t="s" s="4" r="A53">
+    <row r="53" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="4" r="B53">
+      <c r="B53" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54">
-      <c t="s" s="4" r="B54">
+    <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B54" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55">
-      <c t="s" s="4" r="B55">
+    <row r="55" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B55" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="56">
-      <c t="s" s="4" r="B56">
+    <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B56" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57">
-      <c t="s" s="4" r="B57">
+    <row r="57" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B57" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="58">
-      <c t="s" s="4" r="A58">
+    <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>89</v>
       </c>
-      <c t="s" s="4" r="B58">
+      <c r="B58" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="59">
-      <c t="s" s="4" r="B59">
+    <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B59" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="60">
-      <c t="s" s="4" r="B60">
+    <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B60" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="61">
-      <c t="s" s="4" r="B61">
+    <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B61" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="62">
-      <c t="s" s="4" r="B62">
+    <row r="62" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B62" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="63">
-      <c t="s" s="4" r="B63">
+    <row r="63" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B63" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B64" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B65" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="64">
-      <c t="s" s="4" r="A64">
+      <c r="B66" s="3" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="4" r="B64">
+    </row>
+    <row r="67" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B67" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="65">
-      <c t="s" s="4" r="B65">
+    <row r="68" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B68" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="66">
-      <c t="s" s="4" r="B66">
+    <row r="69" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B69" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67">
-      <c t="s" s="4" r="B67">
+    <row r="70" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B70" s="3" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="68">
-      <c t="s" s="4" r="B68">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -852,6 +1166,6 @@
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A2:A13"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DAL download en subfamily gemaakt + getest (etc.)
- SubFamily refactored naar Subfamily. Subfamily is één woord.

- variabele Family family in Subfamily gewijzigd naar int familyId

- mysql connector toegevoegd in de lib folder want driver werd niet
gevonden (zoals bij ons project, Lenny). Nu zit de driver mee in het
project en kunnen geen(?) fouten onstaan.
</commit_message>
<xml_diff>
--- a/Doc/TakenVerdeling/DALmethodes.xlsx
+++ b/Doc/TakenVerdeling/DALmethodes.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lennyasus\Documents\GitHub\ProjectOman\Doc\TakenVerdeling\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5940"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="44">
   <si>
     <t>DAL klasse</t>
   </si>
@@ -145,13 +143,19 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>lenny/Oualid</t>
+  </si>
+  <si>
+    <t>Oualid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -198,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -208,16 +212,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -272,7 +305,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,7 +340,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -484,28 +517,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,8 +554,8 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -537,8 +570,8 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
@@ -551,8 +584,8 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A4" s="9"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
@@ -563,8 +596,8 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A5" s="9"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
@@ -575,8 +608,8 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
@@ -587,8 +620,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A7" s="9"/>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
@@ -599,8 +632,8 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A8" s="9"/>
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
@@ -611,8 +644,8 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A9" s="9"/>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -623,8 +656,8 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A10" s="9"/>
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
@@ -635,8 +668,8 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
@@ -647,8 +680,8 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A12" s="9"/>
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
@@ -659,8 +692,8 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
@@ -671,8 +704,8 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -687,8 +720,8 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A15" s="9"/>
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
@@ -701,8 +734,8 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
@@ -715,8 +748,8 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A17" s="9"/>
       <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
@@ -729,8 +762,8 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A18" s="9"/>
       <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
@@ -743,8 +776,8 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A19" s="9"/>
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
@@ -757,8 +790,8 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A20" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -773,8 +806,8 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A21" s="9"/>
       <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
@@ -787,8 +820,8 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A22" s="9"/>
       <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
@@ -801,8 +834,8 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A23" s="9"/>
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
@@ -815,8 +848,8 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A24" s="9"/>
       <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
@@ -829,70 +862,94 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A25" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="C25" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A26" s="9"/>
       <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="C26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A27" s="9"/>
       <c r="B27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="C27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A28" s="9"/>
       <c r="B28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="C28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A29" s="9"/>
       <c r="B29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="C29" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A30" s="9"/>
       <c r="B30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="C30" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A31" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -903,8 +960,8 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A32" s="9"/>
       <c r="B32" s="3" t="s">
         <v>8</v>
       </c>
@@ -913,8 +970,8 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A33" s="9"/>
       <c r="B33" s="3" t="s">
         <v>22</v>
       </c>
@@ -923,8 +980,8 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A34" s="9"/>
       <c r="B34" s="3" t="s">
         <v>17</v>
       </c>
@@ -933,8 +990,8 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A35" s="9"/>
       <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
@@ -943,8 +1000,8 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A36" s="9"/>
       <c r="B36" s="3" t="s">
         <v>19</v>
       </c>
@@ -953,70 +1010,94 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A37" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="C37" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A38" s="9"/>
       <c r="B38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="C38" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="8"/>
+    <row r="39" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A39" s="9"/>
       <c r="B39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="C39" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
+    <row r="40" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A40" s="9"/>
       <c r="B40" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="C40" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
+    <row r="41" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A41" s="9"/>
       <c r="B41" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="C41" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
+    <row r="42" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A42" s="9"/>
       <c r="B42" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="C42" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A43" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -1031,8 +1112,8 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
+    <row r="44" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A44" s="9"/>
       <c r="B44" s="3" t="s">
         <v>8</v>
       </c>
@@ -1045,8 +1126,8 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
+    <row r="45" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A45" s="9"/>
       <c r="B45" s="3" t="s">
         <v>17</v>
       </c>
@@ -1059,8 +1140,8 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
+    <row r="46" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A46" s="9"/>
       <c r="B46" s="3" t="s">
         <v>18</v>
       </c>
@@ -1073,8 +1154,8 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
+    <row r="47" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A47" s="9"/>
       <c r="B47" s="3" t="s">
         <v>19</v>
       </c>
@@ -1087,8 +1168,8 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A48" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -1099,8 +1180,8 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="8"/>
+    <row r="49" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A49" s="9"/>
       <c r="B49" s="4" t="s">
         <v>13</v>
       </c>
@@ -1109,8 +1190,8 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
+    <row r="50" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A50" s="9"/>
       <c r="B50" s="3" t="s">
         <v>8</v>
       </c>
@@ -1119,8 +1200,8 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="8"/>
+    <row r="51" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A51" s="9"/>
       <c r="B51" s="3" t="s">
         <v>17</v>
       </c>
@@ -1129,8 +1210,8 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
+    <row r="52" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A52" s="9"/>
       <c r="B52" s="3" t="s">
         <v>18</v>
       </c>
@@ -1139,8 +1220,8 @@
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="8"/>
+    <row r="53" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A53" s="9"/>
       <c r="B53" s="3" t="s">
         <v>19</v>
       </c>
@@ -1149,8 +1230,8 @@
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
+    <row r="54" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A54" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -1161,8 +1242,8 @@
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="8"/>
+    <row r="55" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A55" s="9"/>
       <c r="B55" s="3" t="s">
         <v>8</v>
       </c>
@@ -1171,8 +1252,8 @@
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
+    <row r="56" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A56" s="9"/>
       <c r="B56" s="3" t="s">
         <v>17</v>
       </c>
@@ -1181,8 +1262,8 @@
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="8"/>
+    <row r="57" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A57" s="9"/>
       <c r="B57" s="3" t="s">
         <v>18</v>
       </c>
@@ -1191,8 +1272,8 @@
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="8"/>
+    <row r="58" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A58" s="9"/>
       <c r="B58" s="3" t="s">
         <v>19</v>
       </c>
@@ -1201,8 +1282,8 @@
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
+    <row r="59" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A59" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -1217,13 +1298,13 @@
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="8"/>
+    <row r="60" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A60" s="9"/>
       <c r="B60" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>37</v>
+      <c r="C60" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>41</v>
@@ -1231,8 +1312,8 @@
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="8"/>
+    <row r="61" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A61" s="9"/>
       <c r="B61" s="3" t="s">
         <v>17</v>
       </c>
@@ -1245,8 +1326,8 @@
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="8"/>
+    <row r="62" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A62" s="9"/>
       <c r="B62" s="3" t="s">
         <v>18</v>
       </c>
@@ -1259,8 +1340,8 @@
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="8"/>
+    <row r="63" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A63" s="9"/>
       <c r="B63" s="3" t="s">
         <v>19</v>
       </c>
@@ -1273,8 +1354,8 @@
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
     </row>
-    <row r="64" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="8"/>
+    <row r="64" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A64" s="9"/>
       <c r="B64" s="3" t="s">
         <v>34</v>
       </c>
@@ -1287,8 +1368,8 @@
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
     </row>
-    <row r="65" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="8"/>
+    <row r="65" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A65" s="9"/>
       <c r="B65" s="3" t="s">
         <v>39</v>
       </c>
@@ -1301,8 +1382,8 @@
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="8"/>
+    <row r="66" spans="1:6" s="5" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A66" s="9"/>
       <c r="B66" s="3" t="s">
         <v>40</v>
       </c>
@@ -1315,8 +1396,8 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="8"/>
+    <row r="67" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A67" s="9"/>
       <c r="B67" s="6" t="s">
         <v>38</v>
       </c>
@@ -1329,8 +1410,8 @@
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="7" t="s">
+    <row r="68" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A68" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -1341,8 +1422,8 @@
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="8"/>
+    <row r="69" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A69" s="9"/>
       <c r="B69" s="3" t="s">
         <v>8</v>
       </c>
@@ -1351,8 +1432,8 @@
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="8"/>
+    <row r="70" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A70" s="9"/>
       <c r="B70" s="3" t="s">
         <v>22</v>
       </c>
@@ -1361,8 +1442,8 @@
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="8"/>
+    <row r="71" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A71" s="9"/>
       <c r="B71" s="3" t="s">
         <v>17</v>
       </c>
@@ -1371,8 +1452,8 @@
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="8"/>
+    <row r="72" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A72" s="9"/>
       <c r="B72" s="3" t="s">
         <v>18</v>
       </c>
@@ -1381,8 +1462,8 @@
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="8"/>
+    <row r="73" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A73" s="9"/>
       <c r="B73" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
DAL geolocation gemaakt + getest (no coordinates)
</commit_message>
<xml_diff>
--- a/Doc/TakenVerdeling/DALmethodes.xlsx
+++ b/Doc/TakenVerdeling/DALmethodes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="45">
   <si>
     <t>DAL klasse</t>
   </si>
@@ -520,7 +520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -958,8 +958,12 @@
       <c r="B31" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="C31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
@@ -968,8 +972,12 @@
       <c r="B32" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="C32" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
@@ -978,8 +986,12 @@
       <c r="B33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="C33" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
@@ -988,8 +1000,12 @@
       <c r="B34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="C34" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
@@ -998,8 +1014,12 @@
       <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="C35" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
@@ -1008,8 +1028,12 @@
       <c r="B36" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="C36" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>

</xml_diff>